<commit_message>
added xlsx example of mixed inline and not inline country data
</commit_message>
<xml_diff>
--- a/tests/data/full_country_data.xlsx
+++ b/tests/data/full_country_data.xlsx
@@ -3,16 +3,15 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="10776" yWindow="1128" windowWidth="12264" windowHeight="8616" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12576" windowWidth="23256" xWindow="-108" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="time_A" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="time_B" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="power_A" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="power_B" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="changes" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="metadata" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="changes" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="metadata" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -83,90 +82,22 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -471,10 +402,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A6" sqref="A6:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
@@ -492,85 +423,90 @@
       </c>
       <c r="C1" s="4" t="inlineStr">
         <is>
+          <t>country</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
           <t>type</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>param</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>ref value</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>mean growth</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>initial_value_proportional_variation</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>variability growth</t>
         </is>
       </c>
-      <c r="I1" s="4" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>ref date</t>
         </is>
       </c>
-      <c r="J1" s="5" t="inlineStr">
+      <c r="K1" s="5" t="inlineStr">
         <is>
           <t>unit</t>
         </is>
       </c>
-      <c r="K1" s="4" t="inlineStr">
+      <c r="L1" s="4" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
-      <c r="L1" s="4" t="inlineStr">
+      <c r="M1" s="4" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="M1" s="4" t="inlineStr">
+      <c r="N1" s="4" t="inlineStr">
         <is>
           <t>comment</t>
         </is>
       </c>
-      <c r="N1" s="4" t="inlineStr">
+      <c r="O1" s="4" t="inlineStr">
         <is>
           <t>control</t>
         </is>
       </c>
-      <c r="O1" s="4" t="inlineStr">
+      <c r="P1" s="4" t="inlineStr">
         <is>
           <t>scenario notes</t>
         </is>
       </c>
-      <c r="P1" s="5" t="inlineStr">
+      <c r="Q1" s="5" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="Q1" s="4" t="inlineStr">
+      <c r="R1" s="4" t="inlineStr">
         <is>
           <t>ui variable</t>
         </is>
       </c>
-      <c r="R1" s="5" t="inlineStr">
+      <c r="S1" s="5" t="inlineStr">
         <is>
           <t>user name</t>
         </is>
       </c>
-      <c r="S1" s="6" t="inlineStr">
+      <c r="T1" s="6" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -582,54 +518,54 @@
           <t>power_A</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>interp</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>linear</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>{"2020-01-01":10, "2031-06-01":9.5}</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
       <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
         <v>4</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>0.05</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="J2" s="2" t="n">
         <v>43617</v>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>W</t>
         </is>
       </c>
-      <c r="P2" s="3" t="inlineStr">
+      <c r="Q2" s="3" t="inlineStr">
         <is>
           <t>what does it mean? How do collect this info?</t>
         </is>
       </c>
-      <c r="Q2" s="3" t="inlineStr">
+      <c r="R2" s="3" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="R2" s="3" t="inlineStr">
+      <c r="S2" s="3" t="inlineStr">
         <is>
           <t>power draw of laptop</t>
         </is>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -639,44 +575,44 @@
           <t>time_A</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>interp</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>linear</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>{"2020-01-01":100, "2031-06-01":95}</t>
         </is>
       </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
       <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
         <v>5</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>0.05</v>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="J3" s="2" t="n">
         <v>43617</v>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>minute</t>
         </is>
       </c>
-      <c r="Q3" s="3" t="inlineStr">
+      <c r="R3" s="3" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -686,54 +622,54 @@
           <t>power_B</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>interp</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>linear</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>{"2020-01-01":10, "2031-06-01":9.5}</t>
         </is>
       </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
       <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
         <v>4</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>0.05</v>
       </c>
-      <c r="I4" s="2" t="n">
+      <c r="J4" s="2" t="n">
         <v>43617</v>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>W</t>
         </is>
       </c>
-      <c r="P4" s="3" t="inlineStr">
+      <c r="Q4" s="3" t="inlineStr">
         <is>
           <t>what does it mean? How do collect this info?</t>
         </is>
       </c>
-      <c r="Q4" s="3" t="inlineStr">
+      <c r="R4" s="3" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="R4" s="3" t="inlineStr">
+      <c r="S4" s="3" t="inlineStr">
         <is>
           <t>power draw of laptop</t>
         </is>
       </c>
-      <c r="S4" t="n">
+      <c r="T4" t="n">
         <v>2</v>
       </c>
     </row>
@@ -743,55 +679,153 @@
           <t>time_B</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>interp</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>linear</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>{"2020-01-01":100, "2031-06-01":95}</t>
         </is>
       </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
       <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
         <v>5</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>0.05</v>
       </c>
-      <c r="I5" s="2" t="n">
+      <c r="J5" s="2" t="n">
         <v>43617</v>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>minute</t>
         </is>
       </c>
-      <c r="Q5" s="3" t="inlineStr">
+      <c r="R5" s="3" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="S5" t="n">
+      <c r="T5" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="6">
-      <c r="I6" s="2" t="n"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>power_B</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>UK</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>interp</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>{"2020-01-01":100, "2031-06-01":95}</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>43617</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>minute</t>
+        </is>
+      </c>
+      <c r="R6" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="T6" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="7">
-      <c r="I7" s="2" t="n"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>power_B</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>interp</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>{"2020-01-01":100, "2031-06-01":95}</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" t="n">
+        <v>5</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>43617</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>minute</t>
+        </is>
+      </c>
+      <c r="R7" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="T7" t="n">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -803,8 +837,8 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -812,7 +846,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>region</t>
+          <t>country</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -867,7 +901,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="7" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -891,11 +925,11 @@
         <v>0</v>
       </c>
       <c r="G3" s="7" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9" verticalDpi="0"/>
 </worksheet>
 </file>
@@ -909,7 +943,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F3"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -917,7 +951,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>region</t>
+          <t>country</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -972,7 +1006,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="7" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -996,11 +1030,11 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9" verticalDpi="0"/>
 </worksheet>
 </file>
@@ -1014,7 +1048,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -1022,7 +1056,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>region</t>
+          <t>country</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -1077,7 +1111,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -1101,115 +1135,42 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.44140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>region</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>scenario</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>ref value</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>mean growth</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>initial_value_proportional_variation</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>variability growth</t>
-        </is>
-      </c>
-      <c r="G1" s="3" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>UK</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>{"2020-01-01":10, "2031-06-01":9.5}</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>DE</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>{"2020-01-01":10, "2031-06-01":9.5}</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>5</v>
+    <row customHeight="1" ht="15" r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>31.7.18</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>DS change all to lowercase</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -1222,43 +1183,12 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
-  <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>31.7.18</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>DS change all to lowercase</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.44140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>version</t>
@@ -1269,6 +1199,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>